<commit_message>
add: implement overview threshold similarity scores
</commit_message>
<xml_diff>
--- a/backend/phase_one/similarity_scores.xlsx
+++ b/backend/phase_one/similarity_scores.xlsx
@@ -14,15 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
-    <t>C:/Users/Hangsihak Sin/OneDrive/Documents/School/Doc-Wise/backend/phase_one/static/content/temp_files\Hangsihak_Sin_7909104_Assignment4.pdf</t>
+    <t>C:/Users/Hangsihak Sin/OneDrive/Documents/School/Doc-Wise/backend/phase_one/static/content/temp_files\Hangsihak_Sin_Resume.docx</t>
   </si>
   <si>
-    <t>C:/Users/Hangsihak Sin/OneDrive/Documents/School/Doc-Wise/backend/phase_one/static/content/temp_files\Lab3_W23_-_Hangsihak_Sin.pdf</t>
-  </si>
-  <si>
-    <t>C:/Users/Hangsihak Sin/OneDrive/Documents/School/Doc-Wise/backend/phase_one/static/content/temp_files\Lab3_W23_-_Hangsihak_Sin1.pdf</t>
+    <t>C:/Users/Hangsihak Sin/OneDrive/Documents/School/Doc-Wise/backend/phase_one/static/content/temp_files\Hangsihak_Sin_Resume.pdf</t>
   </si>
 </sst>
 </file>
@@ -380,63 +377,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1.000000059604645</v>
+        <v>0.9999999999999996</v>
       </c>
       <c r="C2">
-        <v>0.4396358323854381</v>
-      </c>
-      <c r="D2">
-        <v>0.4407479656499798</v>
+        <v>0.9962553601710249</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.4396358323854381</v>
+        <v>0.9962553601710249</v>
       </c>
       <c r="C3">
-        <v>1.000000059604645</v>
-      </c>
-      <c r="D3">
-        <v>0.9997118115425113</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>0.4407479656499798</v>
-      </c>
-      <c r="C4">
-        <v>0.9997118115425113</v>
-      </c>
-      <c r="D4">
-        <v>1.000000059604645</v>
+        <v>0.9999999403953552</v>
       </c>
     </row>
   </sheetData>

</xml_diff>